<commit_message>
Signed off on Acceptance Test Plan.xlsx sign in requirements.
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\SWEN-261\team-project-2211-swen261-04-h\etc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D08AB7-38CA-4393-821B-CA19C72F02AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="4320" windowWidth="18705" windowHeight="7545" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Instructions</t>
   </si>
@@ -112,11 +118,17 @@
   <si>
     <t>Given that I'm waiting for a game when another player selects a game with me then the system will automatically send me to the Game View as the White player.  NOTE: the `home.ftl` HTML includes a `&lt;meta&gt;` tag that tells the browser to refresh the game every 5 seconds; thus you need to update the `GetHomeRoute` controller to handle the situation when a player is assigned a game.</t>
   </si>
+  <si>
+    <t>AJS &amp; IDC; 10/5/2021</t>
+  </si>
+  <si>
+    <t>AJS &amp; IDC; 10/5/2021; Doesn't display error message, but doesn't allow signin.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -256,6 +268,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -582,7 +597,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -630,12 +645,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H597"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -685,6 +700,9 @@
         <v>5</v>
       </c>
       <c r="C2" s="8"/>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E2" s="8"/>
       <c r="G2" s="8"/>
     </row>
@@ -694,6 +712,9 @@
         <v>25</v>
       </c>
       <c r="C3" s="8"/>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E3" s="8"/>
       <c r="G3" s="8"/>
     </row>
@@ -703,6 +724,9 @@
         <v>24</v>
       </c>
       <c r="C4" s="8"/>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="G4" s="8"/>
     </row>
@@ -712,6 +736,9 @@
         <v>26</v>
       </c>
       <c r="C5" s="8"/>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="G5" s="8"/>
     </row>
@@ -721,6 +748,9 @@
         <v>27</v>
       </c>
       <c r="C6" s="8"/>
+      <c r="D6" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="G6" s="8"/>
     </row>
@@ -730,6 +760,9 @@
         <v>6</v>
       </c>
       <c r="C7" s="8"/>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E7" s="8"/>
       <c r="G7" s="8"/>
     </row>
@@ -739,6 +772,9 @@
         <v>7</v>
       </c>
       <c r="C8" s="8"/>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="G8" s="8"/>
     </row>
@@ -3744,7 +3780,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E597 C2:C597 G2:G597">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E597 C2:C597 G2:G597" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated Acceptance Test Plan to validate Player Sign In
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\SWEN-261\team-project-2211-swen261-04-h\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D08AB7-38CA-4393-821B-CA19C72F02AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F53626-807B-41E4-9B10-9389FFFF95E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5145" yWindow="4320" windowWidth="28800" windowHeight="15345" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Instructions</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>AJS &amp; IDC; 10/5/2021; Doesn't display error message, but doesn't allow signin.</t>
+  </si>
+  <si>
+    <t>AJS; 10/27/2021</t>
+  </si>
+  <si>
+    <t>AJS; 10/28/2021</t>
   </si>
 </sst>
 </file>
@@ -649,8 +655,8 @@
   <dimension ref="A1:H597"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D8" sqref="D8"/>
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -704,6 +710,9 @@
         <v>29</v>
       </c>
       <c r="E2" s="8"/>
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -716,6 +725,9 @@
         <v>29</v>
       </c>
       <c r="E3" s="8"/>
+      <c r="F3" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -728,6 +740,9 @@
         <v>29</v>
       </c>
       <c r="E4" s="8"/>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
@@ -740,6 +755,9 @@
         <v>30</v>
       </c>
       <c r="E5" s="8"/>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -752,6 +770,9 @@
         <v>30</v>
       </c>
       <c r="E6" s="8"/>
+      <c r="F6" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -764,6 +785,9 @@
         <v>29</v>
       </c>
       <c r="E7" s="8"/>
+      <c r="F7" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -776,6 +800,9 @@
         <v>29</v>
       </c>
       <c r="E8" s="8"/>
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
@@ -3771,7 +3798,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D597 F2:F597 H2:H597">
+  <conditionalFormatting sqref="D2:D597 H2:H597 F2:F597">
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
@@ -3785,7 +3812,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated Acceptance Test Plan to validate game start
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\SWEN-261\team-project-2211-swen261-04-h\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F53626-807B-41E4-9B10-9389FFFF95E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1DAA0F-F66C-4AA3-9C7E-1FCF7B92CC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="4320" windowWidth="28800" windowHeight="15345" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Instructions</t>
   </si>
@@ -654,9 +654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H597"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F7" sqref="F7"/>
+      <selection pane="topRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -815,7 +815,9 @@
       <c r="C9" s="12"/>
       <c r="D9" s="11"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="11"/>
     </row>
@@ -826,6 +828,9 @@
       </c>
       <c r="C10" s="8"/>
       <c r="E10" s="8"/>
+      <c r="F10" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="8"/>
     </row>
     <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Players that are already in a game can no longer be selected - If player tries to select another player that is already in a game they will be given an error message - Updated Acceptance Test Plan validate above changes
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\SWEN-261\team-project-2211-swen261-04-h\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1DAA0F-F66C-4AA3-9C7E-1FCF7B92CC5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E906C7BF-D99A-479F-A049-9A5D69472BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="4320" windowWidth="28800" windowHeight="15345" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Instructions</t>
   </si>
@@ -840,6 +840,9 @@
       </c>
       <c r="C11" s="8"/>
       <c r="E11" s="8"/>
+      <c r="F11" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:8" ht="94.5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Acceptance Test Plan to validate all game start user stories
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\SWEN-261\team-project-2211-swen261-04-h\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E906C7BF-D99A-479F-A049-9A5D69472BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F005FA88-2AFB-44F4-A130-91FA70E0DEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="4320" windowWidth="28800" windowHeight="15345" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
   <si>
     <t>Instructions</t>
   </si>
@@ -173,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -190,11 +190,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -228,6 +237,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -654,9 +675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -852,6 +873,9 @@
       </c>
       <c r="C12" s="8"/>
       <c r="E12" s="8"/>
+      <c r="F12" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -861,6 +885,9 @@
       </c>
       <c r="C13" s="8"/>
       <c r="E13" s="8"/>
+      <c r="F13" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
@@ -870,6 +897,9 @@
       </c>
       <c r="C14" s="8"/>
       <c r="E14" s="8"/>
+      <c r="F14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:8" ht="63" x14ac:dyDescent="0.25">
@@ -879,20 +909,28 @@
       </c>
       <c r="C15" s="8"/>
       <c r="E15" s="8"/>
+      <c r="F15" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="8"/>

</xml_diff>

<commit_message>
Updated incorrect validation in Acceptance Test Plan - When dragging a piece to a white space the piece acts as if it is droppable, but fails to drop. - The piece should not be droppable at all.
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\SWEN-261\team-project-2211-swen261-04-h\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F005FA88-2AFB-44F4-A130-91FA70E0DEF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC1D673-7C62-499E-BB81-2BFE853241FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5145" yWindow="4320" windowWidth="28800" windowHeight="15345" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Instructions</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>AJS; 10/28/2021</t>
+  </si>
+  <si>
+    <t>AJS; 10/28/2021; This is sort of works. The space will light up as if it is droppable; however, it will not move when dropped. However, I consider this test failed.</t>
   </si>
 </sst>
 </file>
@@ -255,7 +258,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -675,9 +692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H597"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -878,7 +895,7 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="2" t="s">
         <v>11</v>
@@ -886,7 +903,7 @@
       <c r="C13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G13" s="8"/>
     </row>
@@ -3837,19 +3854,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C597 E2:E597 G2:G597">
-    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D597 H2:H597 F2:F597">
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:D597 H2:H597 F2:F12 F18:F597 F14:F16">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="expression" dxfId="1" priority="15" stopIfTrue="1">
+      <formula>AND(ISBLANK(F13),E17="Pass")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="16" stopIfTrue="1">
+      <formula>AND(ISBLANK(F13),E17="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>